<commit_message>
getting weekly sales done
</commit_message>
<xml_diff>
--- a/Sheet/tfoot.xlsx
+++ b/Sheet/tfoot.xlsx
@@ -551,62 +551,62 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Итог: 17139829.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Итог: 1397126.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Итог: 0.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Итог: 0.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Итог: 17139829.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Итог: 0.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Итог: 0.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Итог: 9149000.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Итог: 0.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Итог: 18536568.00</t>
+          <t>Итог: 0</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>9149000.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>9387568.00</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U2" t="inlineStr"/>

</xml_diff>